<commit_message>
Added new data points from patrick
</commit_message>
<xml_diff>
--- a/DataList.xlsx
+++ b/DataList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="17120" yWindow="0" windowWidth="11680" windowHeight="15720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="251">
   <si>
     <t>Name</t>
   </si>
@@ -675,9 +675,6 @@
     <t>insturl</t>
   </si>
   <si>
-    <t>Institution URL</t>
-  </si>
-  <si>
     <t>vet_tuition_policy_url</t>
   </si>
   <si>
@@ -748,6 +745,33 @@
   </si>
   <si>
     <t>complaints_job_by_fac_code</t>
+  </si>
+  <si>
+    <t>va_highest_degree_offered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">retention_rate_veteran_ba      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">retention_all_students_ba       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">retention_rate_veteran_otb     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">retention_all_students_otb      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">persistance_rate_veteran_ba   </t>
+  </si>
+  <si>
+    <t>persistance_rate_veteran_otb</t>
+  </si>
+  <si>
+    <t>Institution URL, can have "null"</t>
+  </si>
+  <si>
+    <t>Past Columns</t>
   </si>
 </sst>
 </file>
@@ -811,8 +835,60 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="203">
+  <cellStyleXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1028,7 +1104,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="203">
+  <cellStyles count="255">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1130,6 +1206,32 @@
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1231,6 +1333,32 @@
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1562,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1731,12 +1859,12 @@
         <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>218</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>9</v>
@@ -1744,18 +1872,21 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="4" t="s">
-        <v>221</v>
-      </c>
       <c r="B17" s="2" t="s">
-        <v>215</v>
+        <v>9</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1768,13 +1899,13 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1869,7 +2000,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>214</v>
@@ -1877,7 +2008,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>214</v>
@@ -1885,7 +2016,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>214</v>
@@ -1893,311 +2024,302 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="1" t="s">
-        <v>228</v>
+      <c r="A33" s="4" t="s">
+        <v>242</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>230</v>
-      </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="1" t="s">
-        <v>229</v>
+      <c r="A34" s="4" t="s">
+        <v>243</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="1" t="s">
-        <v>231</v>
+      <c r="A35" s="4" t="s">
+        <v>244</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="1" t="s">
-        <v>232</v>
+      <c r="A36" s="4" t="s">
+        <v>245</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="1" t="s">
-        <v>233</v>
+      <c r="A37" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="16" customHeight="1">
-      <c r="A38" s="1" t="s">
-        <v>235</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="1" t="s">
-        <v>234</v>
+      <c r="A39" s="4" t="s">
+        <v>248</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="4" t="s">
-        <v>28</v>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="16" customHeight="1">
+      <c r="A42" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="4" t="s">
-        <v>32</v>
+      <c r="A43" s="1" t="s">
+        <v>233</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F43" s="2" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="4" t="s">
-        <v>33</v>
+      <c r="A44" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="4" t="s">
-        <v>34</v>
+      <c r="A45" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C47" s="2" t="b">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C51" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="4" t="s">
+    <row r="53" spans="1:6">
+      <c r="A53" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="4" t="s">
+      <c r="B53" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="4" t="s">
+    <row r="55" spans="1:6">
+      <c r="A55" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="4" t="s">
+      <c r="B55" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C52" s="2" t="b">
+      <c r="C56" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="4" t="s">
+    <row r="57" spans="1:6">
+      <c r="A57" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="4" t="s">
+    <row r="58" spans="1:6">
+      <c r="A58" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="1" t="s">
+    <row r="59" spans="1:6">
+      <c r="A59" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C59" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C55" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B56" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="4" t="s">
+    <row r="61" spans="1:6">
+      <c r="A61" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="4" t="s">
+      <c r="B61" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="4" t="s">
+      <c r="B62" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="4" t="s">
+      <c r="B63" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>215</v>
@@ -2205,7 +2327,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>215</v>
@@ -2213,7 +2335,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>215</v>
@@ -2221,7 +2343,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="4" t="s">
-        <v>242</v>
+        <v>50</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>215</v>
@@ -2229,7 +2351,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>215</v>
@@ -2237,7 +2359,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>215</v>
@@ -2245,7 +2367,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>215</v>
@@ -2253,7 +2375,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="4" t="s">
-        <v>57</v>
+        <v>241</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>215</v>
@@ -2261,7 +2383,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>215</v>
@@ -2269,7 +2391,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>215</v>
@@ -2277,7 +2399,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>215</v>
@@ -2285,15 +2407,15 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="14" customHeight="1">
+    <row r="76" spans="1:2">
       <c r="A76" s="4" t="s">
-        <v>206</v>
+        <v>58</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>215</v>
@@ -2301,7 +2423,7 @@
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="4" t="s">
-        <v>205</v>
+        <v>59</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>215</v>
@@ -2309,7 +2431,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="4" t="s">
-        <v>207</v>
+        <v>60</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>215</v>
@@ -2317,69 +2439,115 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="14" customHeight="1">
+      <c r="A80" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="4" t="s">
+      <c r="B83" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="4" t="s">
+      <c r="B84" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="4" t="s">
+      <c r="B85" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="3"/>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="3"/>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="3"/>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="3"/>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="B86" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" s="3"/>
     </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="3"/>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="3"/>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="3"/>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="3"/>
-    </row>
-    <row r="93" spans="1:2">
+    <row r="89" spans="1:6" s="1" customFormat="1">
+      <c r="A89" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" s="3" t="s">
         <v>25</v>
       </c>
@@ -2387,7 +2555,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:6">
       <c r="A94" s="3" t="s">
         <v>26</v>
       </c>
@@ -2395,7 +2563,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:6">
       <c r="A95" s="3" t="s">
         <v>27</v>
       </c>
@@ -2403,7 +2571,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:6">
       <c r="A96" s="3" t="s">
         <v>29</v>
       </c>

</xml_diff>